<commit_message>
Deploying to gh-pages from @ Healthedata1/hl7ig-test-build@4ff74fe5ce52f70e84b7bb757c8a80838773f5eb 🚀
</commit_message>
<xml_diff>
--- a/observations-summary.xlsx
+++ b/observations-summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Profile</t>
   </si>
@@ -45,30 +45,6 @@
   </si>
   <si>
     <t>Method</t>
-  </si>
-  <si>
-    <t>pediatric-weight-for-height</t>
-  </si>
-  <si>
-    <t>US Core Pediatric Weight for Height Observation Profile</t>
-  </si>
-  <si>
-    <t>null#vital-signs</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>LOINC#77606-2</t>
-  </si>
-  <si>
-    <t>dateTimeĵ, Periodĵ</t>
-  </si>
-  <si>
-    <t>Quantityĵ, CodeableConceptĵ, stringĵ, booleanĵ, integerĵ, Rangeĵ, Ratioĵ, SampledDataĵ, timeĵ, dateTimeĵ, Periodĵ</t>
-  </si>
-  <si>
-    <t>optional</t>
   </si>
 </sst>
 </file>
@@ -202,7 +178,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -243,41 +219,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="K2" t="s" s="2">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>